<commit_message>
Updates to report to have fit nlogn line
</commit_message>
<xml_diff>
--- a/merge_sort_averages_6.xlsx
+++ b/merge_sort_averages_6.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aejen\Documents\GitHub\MergeSort-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D9B828-94AA-47E4-9D36-8E1FC04371D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1983E79-9373-407B-8775-979570C985FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4572" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="15">
   <si>
     <t>Algorithm</t>
   </si>
@@ -62,6 +75,9 @@
   </si>
   <si>
     <t>nlogn</t>
+  </si>
+  <si>
+    <t>Logarithmic Scale</t>
   </si>
 </sst>
 </file>
@@ -138,12 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -157,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -282,27 +301,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,27 +388,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,27 +475,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,27 +562,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,6 +618,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-F6B5-42A0-84AD-D367217BB2EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E5E-416A-9040-4BFC63455231}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -646,7 +725,25 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:t> Size (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1031,30 +1128,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$C$68</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1121,30 +1215,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$C$68</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1211,30 +1302,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$C$68</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,30 +1389,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$62:$C$68</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,6 +1445,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F552-41D8-AE88-BA47951EFC3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04AE-4065-B182-AF7DB32DDBB1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1402,14 +1547,60 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="-25000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1792,27 +1983,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1879,27 +2070,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1966,27 +2157,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2053,27 +2244,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,6 +2300,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-CCFB-4F2A-9EC5-266D8BF70098}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0436-422D-B64D-FCBB789B3D6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2151,14 +2402,42 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2543,27 +2822,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2630,27 +2909,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2717,27 +2996,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2804,27 +3083,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2860,6 +3139,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ADD4-4A7C-B182-4FFE8E1BD143}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5ED-499B-A9E2-B864379AA70E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2902,14 +3241,42 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3292,27 +3659,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3379,27 +3746,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3466,27 +3833,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3553,27 +3920,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3609,6 +3976,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-57DD-4DBC-8B51-6671F0C259FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>95.000299999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0143-442D-A9FA-D68D47242AF6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3651,14 +4078,42 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4025,27 +4480,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4112,27 +4567,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4199,27 +4654,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4286,27 +4741,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4342,6 +4797,57 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-79E8-478F-9D87-0A656E08F8DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>95.000299999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3393-4489-9821-E7797108372B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4384,14 +4890,42 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4690,27 +5224,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4777,27 +5311,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4864,27 +5398,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4951,27 +5485,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5007,6 +5541,57 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3483-461B-8F5B-DB1781C05EB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>95.000299999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A857-4924-A880-DE2A8D19A4CF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5049,14 +5634,42 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5355,27 +5968,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5442,27 +6055,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5529,27 +6142,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5616,27 +6229,27 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$13</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5672,6 +6285,57 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-52F5-40C3-9236-40A6D0CCF421}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nlogn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>95.000299999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8439-4984-B3CE-E7395BDACC93}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5714,14 +6378,34 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Array</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Array Size (</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>n)</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -8717,16 +9401,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8753,16 +9437,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8791,16 +9475,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>306705</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>59055</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1905</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>363855</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8829,16 +9513,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>150495</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>512445</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>455295</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>207645</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8867,16 +9551,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>268605</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>20955</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>573405</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>325755</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8905,16 +9589,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>140970</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>445770</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8943,16 +9627,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8981,16 +9665,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9309,8 +9993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U78" sqref="U78"/>
+    <sheetView tabSelected="1" topLeftCell="I40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y74" sqref="Y74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9320,9 +10004,12 @@
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9341,8 +10028,12 @@
       <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -9359,10 +10050,15 @@
         <v>96.863476562499997</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <f>0.00000015*$C2*LOG10($C2)</f>
+        <v>1.5E-6</v>
+      </c>
+      <c r="G2">
+        <f>LOG10($C2)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -9379,10 +10075,15 @@
         <v>101.26503906249999</v>
       </c>
       <c r="F3">
-        <v>200</v>
+        <f t="shared" ref="F3:F7" si="0">0.00000015*$C3*LOG10($C3)</f>
+        <v>2.9999999999999997E-5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">LOG10($C3)</f>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -9399,10 +10100,15 @@
         <v>103.24187499999999</v>
       </c>
       <c r="F4">
-        <v>3000</v>
+        <f t="shared" si="0"/>
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -9419,10 +10125,15 @@
         <v>106.714765625</v>
       </c>
       <c r="F5">
-        <v>40000</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9439,10 +10150,15 @@
         <v>130.891484375</v>
       </c>
       <c r="F6">
-        <v>500000</v>
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -9459,10 +10175,15 @@
         <v>353.33011718749998</v>
       </c>
       <c r="F7">
-        <v>6000000</v>
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -9478,8 +10199,12 @@
       <c r="E8">
         <v>96.769101562499998</v>
       </c>
+      <c r="F8">
+        <f>0.00003*$C8*LOG10($C8)+95</f>
+        <v>95.000299999999996</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -9495,8 +10220,12 @@
       <c r="E9">
         <v>101.05140625</v>
       </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F13" si="2">0.00003*$C9*LOG10($C9)+95</f>
+        <v>95.006</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -9512,8 +10241,12 @@
       <c r="E10">
         <v>103.018984375</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>95.09</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -9529,8 +10262,12 @@
       <c r="E11">
         <v>106.38082031250001</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>96.2</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -9546,8 +10283,12 @@
       <c r="E12">
         <v>129.91386718749999</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -9563,8 +10304,12 @@
       <c r="E13">
         <v>292.51164062499998</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>275</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -9581,7 +10326,7 @@
         <v>96.790546875000004</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -9598,7 +10343,7 @@
         <v>101.1971875</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>

</xml_diff>